<commit_message>
converted to desktop application
</commit_message>
<xml_diff>
--- a/Inventory/data.xlsx
+++ b/Inventory/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>uniqueId</t>
   </si>
@@ -49,31 +49,73 @@
     <t>product1</t>
   </si>
   <si>
-    <t>afw</t>
-  </si>
-  <si>
-    <t>af</t>
-  </si>
-  <si>
-    <t>2022-03-01</t>
-  </si>
-  <si>
-    <t>2022-03-02</t>
-  </si>
-  <si>
-    <t>2022-03-08</t>
-  </si>
-  <si>
-    <t>2022-03-09</t>
-  </si>
-  <si>
-    <t>2022-03-04</t>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>p3</t>
+  </si>
+  <si>
+    <t>p4</t>
+  </si>
+  <si>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>p6</t>
+  </si>
+  <si>
+    <t>afwa</t>
+  </si>
+  <si>
+    <t>prod</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>2022-03-24</t>
+  </si>
+  <si>
+    <t>2022-03-17</t>
+  </si>
+  <si>
+    <t>2022-03-16</t>
+  </si>
+  <si>
+    <t>2022-03-14</t>
+  </si>
+  <si>
+    <t>2022-03-23</t>
+  </si>
+  <si>
+    <t>2022-03-15</t>
+  </si>
+  <si>
+    <t>1222-12-02</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
   <si>
     <t>fawaf</t>
   </si>
   <si>
-    <t>xyz</t>
+    <t>firmname</t>
+  </si>
+  <si>
+    <t>fawfwa</t>
+  </si>
+  <si>
+    <t>grsrsg</t>
+  </si>
+  <si>
+    <t>gsggegs</t>
+  </si>
+  <si>
+    <t>egs</t>
+  </si>
+  <si>
+    <t>fawf</t>
   </si>
 </sst>
 </file>
@@ -431,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,7 +510,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2">
-        <v>335399081</v>
+        <v>423971248</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -477,27 +519,27 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G2">
-        <v>199</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>300</v>
       </c>
       <c r="I2">
-        <v>200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
-        <v>1</v>
+        <v>187616088</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -506,48 +548,48 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>123</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G3">
-        <v>199</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="I3">
-        <v>2400</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4">
-        <v>282165193</v>
+        <v>306070755</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E4">
         <v>123</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="G4">
-        <v>199</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="I4">
         <v>200</v>
@@ -555,263 +597,205 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
-        <v>823432304</v>
+        <v>87968817</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E5">
-        <v>123</v>
+        <v>2222</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G5">
-        <v>199</v>
+        <v>7</v>
       </c>
       <c r="H5">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="I5">
-        <v>200</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6">
-        <v>901183918</v>
+        <v>961795813</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E6">
-        <v>123</v>
+        <v>555</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="G6">
-        <v>199</v>
+        <v>7</v>
       </c>
       <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
         <v>300</v>
-      </c>
-      <c r="I6">
-        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7">
-        <v>510172359</v>
+        <v>608870061</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>123</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G7">
-        <v>199</v>
+        <v>8</v>
       </c>
       <c r="H7">
         <v>300</v>
       </c>
       <c r="I7">
-        <v>200</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
-        <v>984823139</v>
+        <v>386861217</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E8">
-        <v>123</v>
+        <v>23114</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="G8">
-        <v>199</v>
+        <v>7</v>
       </c>
       <c r="H8">
-        <v>300</v>
+        <v>1344</v>
       </c>
       <c r="I8">
-        <v>200</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9">
-        <v>826639299</v>
+        <v>768040092</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E9">
-        <v>123</v>
+        <v>1233</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="G9">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="H9">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="I9">
-        <v>200</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10">
-        <v>66059634</v>
+        <v>885174910</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E10">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G10">
-        <v>199</v>
+        <v>6</v>
       </c>
       <c r="H10">
-        <v>300</v>
+        <v>5223</v>
       </c>
       <c r="I10">
-        <v>200</v>
+        <v>15624</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11">
-        <v>337062910</v>
+        <v>191385747</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E11">
+        <v>1234</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
         <v>123</v>
       </c>
-      <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11">
-        <v>300</v>
-      </c>
       <c r="I11">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
-        <v>875594548</v>
-      </c>
-      <c r="B12" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12">
-        <v>123</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12">
-        <v>199</v>
-      </c>
-      <c r="H12">
-        <v>300</v>
-      </c>
-      <c r="I12">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13">
-        <v>487817572</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13">
-        <v>123</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G13">
-        <v>199</v>
-      </c>
-      <c r="H13">
-        <v>300</v>
-      </c>
-      <c r="I13">
-        <v>200</v>
+        <v>5235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>